<commit_message>
Update performance price analysis
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/performance/Performance-Graphs.xlsx
+++ b/documents/resources/evaluation/performance/Performance-Graphs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>INDY2</t>
   </si>
@@ -34,6 +34,27 @@
   </si>
   <si>
     <t>Simulation total time in second</t>
+  </si>
+  <si>
+    <t>#Compute node</t>
+  </si>
+  <si>
+    <t>Perf Delta</t>
+  </si>
+  <si>
+    <t>Total partner price diff</t>
+  </si>
+  <si>
+    <t>Total non-partner price diff</t>
+  </si>
+  <si>
+    <t>Simulation time</t>
+  </si>
+  <si>
+    <t>Price delta / node (Partner)</t>
+  </si>
+  <si>
+    <t>Price delta / node (NonPartner)</t>
   </si>
 </sst>
 </file>
@@ -82,8 +103,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -125,7 +176,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -143,6 +194,21 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -160,6 +226,21 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,16 +662,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -934,22 +1015,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E16"/>
+  <dimension ref="A2:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:7">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:7">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -963,15 +1050,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:7">
       <c r="B4">
         <v>24</v>
       </c>
       <c r="E4">
         <v>33.6</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="G4">
+        <f>36.3/33.6</f>
+        <v>1.0803571428571428</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5">
         <v>36</v>
       </c>
@@ -982,15 +1073,19 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:7">
       <c r="B6">
         <v>48</v>
       </c>
       <c r="E6">
         <v>22.1</v>
       </c>
-    </row>
-    <row r="7" spans="2:5">
+      <c r="G6">
+        <f>29.9/22.1</f>
+        <v>1.3529411764705881</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7">
         <v>72</v>
       </c>
@@ -1001,15 +1096,19 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:7">
       <c r="B8">
         <v>96</v>
       </c>
       <c r="E8">
         <v>13.4</v>
       </c>
-    </row>
-    <row r="9" spans="2:5">
+      <c r="G8">
+        <f>36.5/13.4</f>
+        <v>2.7238805970149254</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9">
         <v>144</v>
       </c>
@@ -1020,15 +1119,19 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:7">
       <c r="B10">
         <v>192</v>
       </c>
       <c r="E10">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="G10">
+        <f>32.4/9.81</f>
+        <v>3.3027522935779814</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
       <c r="B11">
         <v>288</v>
       </c>
@@ -1039,15 +1142,19 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:7">
       <c r="B12">
         <v>384</v>
       </c>
       <c r="E12">
         <v>9.94</v>
       </c>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="G12">
+        <f>20.4/9.94</f>
+        <v>2.0523138832997989</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
       <c r="B13">
         <v>576</v>
       </c>
@@ -1058,7 +1165,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:7">
       <c r="B14">
         <v>768</v>
       </c>
@@ -1066,7 +1173,7 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:7">
       <c r="B15">
         <v>1152</v>
       </c>
@@ -1074,7 +1181,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:7">
       <c r="B16">
         <v>1536</v>
       </c>
@@ -1082,9 +1189,197 @@
         <v>18.600000000000001</v>
       </c>
     </row>
+    <row r="22" spans="1:8">
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C24">
+        <v>33.6</v>
+      </c>
+      <c r="D24">
+        <f>B24/C24</f>
+        <v>1.0803571428571428</v>
+      </c>
+      <c r="E24">
+        <v>7.55</v>
+      </c>
+      <c r="F24">
+        <f>E24*D24</f>
+        <v>8.1566964285714274</v>
+      </c>
+      <c r="G24">
+        <v>3.14</v>
+      </c>
+      <c r="H24">
+        <f>D24*G24</f>
+        <v>3.3923214285714285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>29.9</v>
+      </c>
+      <c r="C25">
+        <v>22.1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:D28" si="0">B25/C25</f>
+        <v>1.3529411764705881</v>
+      </c>
+      <c r="E25">
+        <v>7.55</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F28" si="1">E25*D25</f>
+        <v>10.21470588235294</v>
+      </c>
+      <c r="G25">
+        <v>3.14</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H28" si="2">D25*G25</f>
+        <v>4.2482352941176469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>36.5</v>
+      </c>
+      <c r="C26">
+        <v>13.4</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.7238805970149254</v>
+      </c>
+      <c r="E26">
+        <v>7.55</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>20.565298507462686</v>
+      </c>
+      <c r="G26">
+        <v>3.14</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>8.5529850746268661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>32.4</v>
+      </c>
+      <c r="C27">
+        <v>9.81</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>3.3027522935779814</v>
+      </c>
+      <c r="E27">
+        <v>7.55</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>24.935779816513758</v>
+      </c>
+      <c r="G27">
+        <v>3.14</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>10.370642201834862</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="C28">
+        <v>9.94</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.0523138832997989</v>
+      </c>
+      <c r="E28">
+        <v>7.55</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>15.494969818913482</v>
+      </c>
+      <c r="G28">
+        <v>3.14</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>6.4442655935613686</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="C29">
+        <v>9.64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="C30">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated performance result with correct CPU count
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/performance/Performance-Graphs.xlsx
+++ b/documents/resources/evaluation/performance/Performance-Graphs.xlsx
@@ -103,8 +103,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -176,7 +192,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -209,6 +225,14 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -241,6 +265,14 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -282,6 +314,25 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="3366FF"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$16</c:f>
@@ -289,43 +340,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>36.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>48.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>96.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>144.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>192.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>288.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>384.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>576.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>768.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1152.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1536.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,22 +387,22 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>24.7</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>12.7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7.08</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3.44</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1.81</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1.58</c:v>
                 </c:pt>
               </c:numCache>
@@ -373,6 +424,25 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$16</c:f>
@@ -380,43 +450,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>36.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>48.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>96.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>144.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>192.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>288.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>384.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>576.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>768.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1152.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1536.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -427,20 +497,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="1">
-                  <c:v>36.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20.4</c:v>
+                <c:pt idx="0">
+                  <c:v>35.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,6 +531,25 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$16</c:f>
@@ -468,43 +557,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>36.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>48.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>96.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>144.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>192.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>288.0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>384.0</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>576.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>768.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1152.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1536.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -515,26 +604,23 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0">
+                <c:pt idx="1">
                   <c:v>33.6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>22.1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>13.4</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>9.81</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9.94</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>9.64</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>18.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,12 +641,14 @@
       <c:valAx>
         <c:axId val="-2146329272"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:max val="1600.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1300.0"/>
+          <c:min val="10.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -572,13 +660,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>#</a:t>
+                  <a:t>Cores (Log)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Cores</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -596,6 +679,7 @@
       <c:valAx>
         <c:axId val="-2141855304"/>
         <c:scaling>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -612,13 +696,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Simulation</a:t>
+                  <a:t>Time  / S  (Log)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> time in seconds</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -636,6 +715,18 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -670,7 +761,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1015,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H30"/>
+  <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1052,10 +1143,10 @@
     </row>
     <row r="4" spans="2:7">
       <c r="B4">
-        <v>24</v>
-      </c>
-      <c r="E4">
-        <v>33.6</v>
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>35.299999999999997</v>
       </c>
       <c r="G4">
         <f>36.3/33.6</f>
@@ -1064,21 +1155,21 @@
     </row>
     <row r="5" spans="2:7">
       <c r="B5">
-        <v>36</v>
-      </c>
-      <c r="C5">
-        <v>24.7</v>
-      </c>
-      <c r="D5">
-        <v>36.299999999999997</v>
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>33.6</v>
       </c>
     </row>
     <row r="6" spans="2:7">
       <c r="B6">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>22.1</v>
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>24.7</v>
+      </c>
+      <c r="D6">
+        <v>24.6</v>
       </c>
       <c r="G6">
         <f>29.9/22.1</f>
@@ -1087,21 +1178,21 @@
     </row>
     <row r="7" spans="2:7">
       <c r="B7">
-        <v>72</v>
-      </c>
-      <c r="C7">
-        <v>12.7</v>
-      </c>
-      <c r="D7">
-        <v>29.9</v>
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>22.1</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8">
-        <v>96</v>
-      </c>
-      <c r="E8">
-        <v>13.4</v>
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>12.7</v>
+      </c>
+      <c r="D8">
+        <v>16.8</v>
       </c>
       <c r="G8">
         <f>36.5/13.4</f>
@@ -1110,21 +1201,21 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9">
-        <v>144</v>
-      </c>
-      <c r="C9">
-        <v>7.08</v>
-      </c>
-      <c r="D9">
-        <v>36.5</v>
+        <v>96</v>
+      </c>
+      <c r="E9">
+        <v>13.4</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10">
-        <v>192</v>
-      </c>
-      <c r="E10">
-        <v>9.81</v>
+        <v>144</v>
+      </c>
+      <c r="C10">
+        <v>7.08</v>
+      </c>
+      <c r="D10">
+        <v>11.5</v>
       </c>
       <c r="G10">
         <f>32.4/9.81</f>
@@ -1133,21 +1224,21 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11">
-        <v>288</v>
-      </c>
-      <c r="C11">
-        <v>3.44</v>
-      </c>
-      <c r="D11">
-        <v>32.4</v>
+        <v>192</v>
+      </c>
+      <c r="E11">
+        <v>9.81</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12">
-        <v>384</v>
-      </c>
-      <c r="E12">
-        <v>9.94</v>
+        <v>288</v>
+      </c>
+      <c r="C12">
+        <v>3.44</v>
+      </c>
+      <c r="D12">
+        <v>10.3</v>
       </c>
       <c r="G12">
         <f>20.4/9.94</f>
@@ -1156,230 +1247,222 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13">
-        <v>576</v>
-      </c>
-      <c r="C13">
-        <v>1.81</v>
-      </c>
-      <c r="D13">
-        <v>20.399999999999999</v>
+        <v>384</v>
+      </c>
+      <c r="E13">
+        <v>9.94</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14">
-        <v>768</v>
-      </c>
-      <c r="E14">
-        <v>9.64</v>
+        <v>576</v>
+      </c>
+      <c r="C14">
+        <v>1.81</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15">
-        <v>1152</v>
-      </c>
-      <c r="C15">
-        <v>1.58</v>
+        <v>768</v>
+      </c>
+      <c r="E15">
+        <v>9.64</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16">
-        <v>1536</v>
-      </c>
-      <c r="E16">
-        <v>18.600000000000001</v>
-      </c>
+        <v>1152</v>
+      </c>
+      <c r="C16">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1"/>
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="A23">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
+      <c r="B23">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C23">
+        <v>33.6</v>
+      </c>
+      <c r="D23">
+        <f>B23/C23</f>
+        <v>1.0803571428571428</v>
+      </c>
+      <c r="E23">
+        <v>7.55</v>
+      </c>
+      <c r="F23">
+        <f>E23*D23</f>
+        <v>8.1566964285714274</v>
+      </c>
+      <c r="G23">
+        <v>3.14</v>
+      </c>
+      <c r="H23">
+        <f>D23*G23</f>
+        <v>3.3923214285714285</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24">
-        <v>36.299999999999997</v>
+        <v>29.9</v>
       </c>
       <c r="C24">
-        <v>33.6</v>
+        <v>22.1</v>
       </c>
       <c r="D24">
-        <f>B24/C24</f>
-        <v>1.0803571428571428</v>
+        <f t="shared" ref="D24:D27" si="0">B24/C24</f>
+        <v>1.3529411764705881</v>
       </c>
       <c r="E24">
         <v>7.55</v>
       </c>
       <c r="F24">
-        <f>E24*D24</f>
-        <v>8.1566964285714274</v>
+        <f t="shared" ref="F24:F27" si="1">E24*D24</f>
+        <v>10.21470588235294</v>
       </c>
       <c r="G24">
         <v>3.14</v>
       </c>
       <c r="H24">
-        <f>D24*G24</f>
-        <v>3.3923214285714285</v>
+        <f t="shared" ref="H24:H27" si="2">D24*G24</f>
+        <v>4.2482352941176469</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25">
-        <v>29.9</v>
+        <v>36.5</v>
       </c>
       <c r="C25">
-        <v>22.1</v>
+        <v>13.4</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:D28" si="0">B25/C25</f>
-        <v>1.3529411764705881</v>
+        <f t="shared" si="0"/>
+        <v>2.7238805970149254</v>
       </c>
       <c r="E25">
         <v>7.55</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:F28" si="1">E25*D25</f>
-        <v>10.21470588235294</v>
+        <f t="shared" si="1"/>
+        <v>20.565298507462686</v>
       </c>
       <c r="G25">
         <v>3.14</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H28" si="2">D25*G25</f>
-        <v>4.2482352941176469</v>
+        <f t="shared" si="2"/>
+        <v>8.5529850746268661</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>36.5</v>
+        <v>32.4</v>
       </c>
       <c r="C26">
-        <v>13.4</v>
+        <v>9.81</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>2.7238805970149254</v>
+        <v>3.3027522935779814</v>
       </c>
       <c r="E26">
         <v>7.55</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>20.565298507462686</v>
+        <v>24.935779816513758</v>
       </c>
       <c r="G26">
         <v>3.14</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>8.5529850746268661</v>
+        <v>10.370642201834862</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>32.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="C27">
-        <v>9.81</v>
+        <v>9.94</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>3.3027522935779814</v>
+        <v>2.0523138832997989</v>
       </c>
       <c r="E27">
         <v>7.55</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>24.935779816513758</v>
+        <v>15.494969818913482</v>
       </c>
       <c r="G27">
         <v>3.14</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>10.370642201834862</v>
+        <v>6.4442655935613686</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="B28">
-        <v>20.399999999999999</v>
-      </c>
       <c r="C28">
-        <v>9.94</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>2.0523138832997989</v>
-      </c>
-      <c r="E28">
-        <v>7.55</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
-        <v>15.494969818913482</v>
-      </c>
-      <c r="G28">
-        <v>3.14</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="2"/>
-        <v>6.4442655935613686</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="C29">
         <v>9.64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="C30">
-        <v>18.600000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B21:C21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added parallel efficiency figure, and added infrastructure description to evaluation
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/performance/Performance-Graphs.xlsx
+++ b/documents/resources/evaluation/performance/Performance-Graphs.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
   <si>
     <t>INDY2</t>
   </si>
@@ -28,6 +29,9 @@
   </si>
   <si>
     <t>AWS-EC2</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>#of Core</t>
@@ -42,19 +46,56 @@
     <t>Perf Delta</t>
   </si>
   <si>
-    <t>Total partner price diff</t>
-  </si>
-  <si>
-    <t>Total non-partner price diff</t>
-  </si>
-  <si>
     <t>Simulation time</t>
   </si>
   <si>
-    <t>Price delta / node (Partner)</t>
+    <t># Compute nodes</t>
   </si>
   <si>
-    <t>Price delta / node (NonPartner)</t>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Time / s</t>
+  </si>
+  <si>
+    <t>Core count</t>
+  </si>
+  <si>
+    <t>Execution time</t>
+  </si>
+  <si>
+    <t>Speed up</t>
+  </si>
+  <si>
+    <t>Efficienc</t>
+  </si>
+  <si>
+    <t>EFFICIENCY</t>
+  </si>
+  <si>
+    <t>EFFICIENCY INDY2</t>
+  </si>
+  <si>
+    <t>Time/s</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>EFFICIENCY  ARCHER</t>
+  </si>
+  <si>
+    <t>EFFICIENCY AWS-EC2</t>
+  </si>
+  <si>
+    <t>Ideal speedup</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>Ideal parallel 
+efficiency</t>
   </si>
 </sst>
 </file>
@@ -94,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -102,8 +143,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -185,14 +316,221 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -233,6 +571,84 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -273,6 +689,84 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -656,11 +1150,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Cores (Log)</a:t>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Cores (Log10)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -692,11 +1186,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time  / S  (Log)</a:t>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Time  / S  (Log10)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -749,6 +1243,527 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>INDY2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$45:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>192.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>384.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1152.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$45:$G$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97244094488189</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.872175141242938</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.897529069767442</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.852900552486188</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.488528481012658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AWS-EC2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$45:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>192.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>384.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1152.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$45:$H$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.717479674796748</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.525297619047619</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.383695652173913</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.214199029126214</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARCHER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$45:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>192.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>384.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>576.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>768.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1152.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$45:$I$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.760180995475113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.626865671641791</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.428134556574924</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.211267605633803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.108921161825726</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal parallel _x000d_efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$45:$J$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$45:$K$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2140565896"/>
+        <c:axId val="-2145111160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2140565896"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1200.0"/>
+          <c:min val="10.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Core</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> (Log10)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2145111160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2145111160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Parallel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140565896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -776,6 +1791,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1106,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H28"/>
+  <dimension ref="A2:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1118,18 +2163,19 @@
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1278,14 +2324,14 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -1294,19 +2340,13 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1314,28 +2354,21 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>36.299999999999997</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="C23">
         <v>33.6</v>
       </c>
       <c r="D23">
         <f>B23/C23</f>
-        <v>1.0803571428571428</v>
+        <v>1.0505952380952379</v>
       </c>
       <c r="E23">
-        <v>7.55</v>
+        <v>24.7</v>
       </c>
       <c r="F23">
-        <f>E23*D23</f>
-        <v>8.1566964285714274</v>
-      </c>
-      <c r="G23">
-        <v>3.14</v>
-      </c>
-      <c r="H23">
-        <f>D23*G23</f>
-        <v>3.3923214285714285</v>
+        <f>B23/E23</f>
+        <v>1.42914979757085</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1343,28 +2376,21 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>29.9</v>
+        <v>24.6</v>
       </c>
       <c r="C24">
         <v>22.1</v>
       </c>
       <c r="D24">
         <f t="shared" ref="D24:D27" si="0">B24/C24</f>
-        <v>1.3529411764705881</v>
+        <v>1.1131221719457014</v>
       </c>
       <c r="E24">
-        <v>7.55</v>
+        <v>12.7</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F27" si="1">E24*D24</f>
-        <v>10.21470588235294</v>
-      </c>
-      <c r="G24">
-        <v>3.14</v>
-      </c>
-      <c r="H24">
-        <f t="shared" ref="H24:H27" si="2">D24*G24</f>
-        <v>4.2482352941176469</v>
+        <f t="shared" ref="F24:F27" si="1">B24/E24</f>
+        <v>1.9370078740157481</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1372,28 +2398,21 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>36.5</v>
+        <v>16.8</v>
       </c>
       <c r="C25">
         <v>13.4</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>2.7238805970149254</v>
+        <v>1.2537313432835822</v>
       </c>
       <c r="E25">
-        <v>7.55</v>
+        <v>7.08</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>20.565298507462686</v>
-      </c>
-      <c r="G25">
-        <v>3.14</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="2"/>
-        <v>8.5529850746268661</v>
+        <v>2.3728813559322033</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1401,28 +2420,21 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>32.4</v>
+        <v>11.5</v>
       </c>
       <c r="C26">
         <v>9.81</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>3.3027522935779814</v>
+        <v>1.1722731906218145</v>
       </c>
       <c r="E26">
-        <v>7.55</v>
+        <v>3.44</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>24.935779816513758</v>
-      </c>
-      <c r="G26">
-        <v>3.14</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="2"/>
-        <v>10.370642201834862</v>
+        <v>3.3430232558139537</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1430,39 +2442,1223 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <v>20.399999999999999</v>
+        <v>10.3</v>
       </c>
       <c r="C27">
         <v>9.94</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>2.0523138832997989</v>
+        <v>1.0362173038229376</v>
       </c>
       <c r="E27">
-        <v>7.55</v>
+        <v>1.81</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>15.494969818913482</v>
-      </c>
-      <c r="G27">
-        <v>3.14</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="2"/>
-        <v>6.4442655935613686</v>
+        <v>5.6906077348066297</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="C28">
         <v>9.64</v>
       </c>
+      <c r="E28">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="12"/>
+      <c r="B33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="9">
+        <v>36</v>
+      </c>
+      <c r="C34" s="5">
+        <v>24.7</v>
+      </c>
+      <c r="D34" s="5">
+        <v>24</v>
+      </c>
+      <c r="E34" s="5">
+        <v>33.6</v>
+      </c>
+      <c r="F34" s="5">
+        <v>18</v>
+      </c>
+      <c r="G34" s="5">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="8">
+        <v>2</v>
+      </c>
+      <c r="B35" s="7">
+        <v>72</v>
+      </c>
+      <c r="C35" s="8">
+        <v>12.7</v>
+      </c>
+      <c r="D35" s="8">
+        <v>48</v>
+      </c>
+      <c r="E35" s="8">
+        <v>22.1</v>
+      </c>
+      <c r="F35" s="8">
+        <v>36</v>
+      </c>
+      <c r="G35" s="8">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="8">
+        <v>3</v>
+      </c>
+      <c r="B36" s="7">
+        <v>144</v>
+      </c>
+      <c r="C36" s="8">
+        <v>7.08</v>
+      </c>
+      <c r="D36" s="8">
+        <v>96</v>
+      </c>
+      <c r="E36" s="8">
+        <v>13.4</v>
+      </c>
+      <c r="F36" s="8">
+        <v>72</v>
+      </c>
+      <c r="G36" s="8">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="8">
+        <v>4</v>
+      </c>
+      <c r="B37" s="7">
+        <v>288</v>
+      </c>
+      <c r="C37" s="8">
+        <v>3.44</v>
+      </c>
+      <c r="D37" s="8">
+        <v>192</v>
+      </c>
+      <c r="E37" s="8">
+        <v>9.81</v>
+      </c>
+      <c r="F37" s="8">
+        <v>144</v>
+      </c>
+      <c r="G37" s="8">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="8">
+        <v>5</v>
+      </c>
+      <c r="B38" s="7">
+        <v>576</v>
+      </c>
+      <c r="C38" s="8">
+        <v>1.81</v>
+      </c>
+      <c r="D38" s="8">
+        <v>384</v>
+      </c>
+      <c r="E38" s="8">
+        <v>9.94</v>
+      </c>
+      <c r="F38" s="8">
+        <v>288</v>
+      </c>
+      <c r="G38" s="8">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="6">
+        <v>6</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1152</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1.58</v>
+      </c>
+      <c r="D39" s="6">
+        <v>768</v>
+      </c>
+      <c r="E39" s="6">
+        <v>9.64</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="G43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" ht="45">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>10</v>
+      </c>
+      <c r="K44" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="9">
+        <v>36</v>
+      </c>
+      <c r="B45" s="5">
+        <v>24.7</v>
+      </c>
+      <c r="C45">
+        <f>$B$45 /B45</f>
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <f>(C45/A45) * $A$45</f>
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>18</v>
+      </c>
+      <c r="H45">
+        <f>D64</f>
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="7">
+        <v>72</v>
+      </c>
+      <c r="B46" s="8">
+        <v>12.7</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:C50" si="2">$B$45 /B46</f>
+        <v>1.9448818897637796</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ref="D46:D50" si="3">(C46/A46) * $A$45</f>
+        <v>0.97244094488188981</v>
+      </c>
+      <c r="F46">
+        <v>24</v>
+      </c>
+      <c r="I46">
+        <f>D55</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="7">
+        <v>144</v>
+      </c>
+      <c r="B47" s="8">
+        <v>7.08</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>3.4887005649717513</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="3"/>
+        <v>0.87217514124293782</v>
+      </c>
+      <c r="F47">
+        <v>36</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <f>D65</f>
+        <v>0.7174796747967479</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="7">
+        <v>288</v>
+      </c>
+      <c r="B48" s="8">
+        <v>3.44</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>7.1802325581395348</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="3"/>
+        <v>0.89752906976744184</v>
+      </c>
+      <c r="F48">
+        <v>48</v>
+      </c>
+      <c r="I48">
+        <f>D56</f>
+        <v>0.76018099547511309</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="7">
+        <v>576</v>
+      </c>
+      <c r="B49" s="8">
+        <v>1.81</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>13.646408839779005</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="3"/>
+        <v>0.85290055248618779</v>
+      </c>
+      <c r="F49">
+        <v>72</v>
+      </c>
+      <c r="G49">
+        <f>D46</f>
+        <v>0.97244094488188981</v>
+      </c>
+      <c r="H49">
+        <f>D66</f>
+        <v>0.52529761904761896</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="10">
+        <v>1152</v>
+      </c>
+      <c r="B50" s="6">
+        <v>1.58</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>15.632911392405061</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="3"/>
+        <v>0.48852848101265817</v>
+      </c>
+      <c r="F50">
+        <v>96</v>
+      </c>
+      <c r="I50">
+        <f>D57</f>
+        <v>0.62686567164179108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="F51">
+        <v>144</v>
+      </c>
+      <c r="G51">
+        <f>D47</f>
+        <v>0.87217514124293782</v>
+      </c>
+      <c r="H51">
+        <f>D67</f>
+        <v>0.38369565217391299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="F52">
+        <v>192</v>
+      </c>
+      <c r="I52">
+        <f>D58</f>
+        <v>0.42813455657492355</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="F53">
+        <v>288</v>
+      </c>
+      <c r="G53">
+        <f>D48</f>
+        <v>0.89752906976744184</v>
+      </c>
+      <c r="H53">
+        <f>D68</f>
+        <v>0.21419902912621355</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54">
+        <v>384</v>
+      </c>
+      <c r="I54">
+        <f>D59</f>
+        <v>0.21126760563380281</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="5">
+        <v>24</v>
+      </c>
+      <c r="B55" s="5">
+        <v>33.6</v>
+      </c>
+      <c r="C55">
+        <f>$B$55 /B55</f>
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <f>(C55/A55) * $A$55</f>
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>576</v>
+      </c>
+      <c r="G55">
+        <f>D49</f>
+        <v>0.85290055248618779</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="8">
+        <v>48</v>
+      </c>
+      <c r="B56" s="8">
+        <v>22.1</v>
+      </c>
+      <c r="C56">
+        <f t="shared" ref="C56:C60" si="4">$B$55 /B56</f>
+        <v>1.5203619909502262</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ref="D56:D60" si="5">(C56/A56) * $A$55</f>
+        <v>0.76018099547511309</v>
+      </c>
+      <c r="F56">
+        <v>768</v>
+      </c>
+      <c r="I56">
+        <f>D60</f>
+        <v>0.10892116182572614</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="8">
+        <v>96</v>
+      </c>
+      <c r="B57" s="8">
+        <v>13.4</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="4"/>
+        <v>2.5074626865671643</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="5"/>
+        <v>0.62686567164179108</v>
+      </c>
+      <c r="F57">
+        <v>1152</v>
+      </c>
+      <c r="G57">
+        <f>D50</f>
+        <v>0.48852848101265817</v>
+      </c>
+      <c r="J57">
+        <v>10000</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="8">
+        <v>192</v>
+      </c>
+      <c r="B58" s="8">
+        <v>9.81</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="4"/>
+        <v>3.4250764525993884</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="5"/>
+        <v>0.42813455657492355</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="8">
+        <v>384</v>
+      </c>
+      <c r="B59" s="8">
+        <v>9.94</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="4"/>
+        <v>3.3802816901408455</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="5"/>
+        <v>0.21126760563380281</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="6">
+        <v>768</v>
+      </c>
+      <c r="B60" s="6">
+        <v>9.64</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="4"/>
+        <v>3.4854771784232366</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="5"/>
+        <v>0.10892116182572614</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="5">
+        <v>18</v>
+      </c>
+      <c r="B64" s="5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C64">
+        <f>$B$64 /B64</f>
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <f>(C64/A64) * $A$64</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="8">
+        <v>36</v>
+      </c>
+      <c r="B65" s="8">
+        <v>24.6</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ref="C65:C69" si="6">$B$64 /B65</f>
+        <v>1.4349593495934958</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ref="D65:D68" si="7">(C65/A65) * $A$64</f>
+        <v>0.7174796747967479</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="8">
+        <v>72</v>
+      </c>
+      <c r="B66" s="8">
+        <v>16.8</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="6"/>
+        <v>2.1011904761904758</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="7"/>
+        <v>0.52529761904761896</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="8">
+        <v>144</v>
+      </c>
+      <c r="B67" s="8">
+        <v>11.5</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="6"/>
+        <v>3.0695652173913039</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="7"/>
+        <v>0.38369565217391299</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="8">
+        <v>288</v>
+      </c>
+      <c r="B68" s="8">
+        <v>10.3</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="6"/>
+        <v>3.4271844660194168</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="7"/>
+        <v>0.21419902912621355</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="F69" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" t="s">
+        <v>0</v>
+      </c>
+      <c r="H69" t="s">
+        <v>2</v>
+      </c>
+      <c r="I69" t="s">
+        <v>1</v>
+      </c>
+      <c r="J69" t="s">
+        <v>10</v>
+      </c>
+      <c r="K69" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="F70">
+        <v>18</v>
+      </c>
+      <c r="H70">
+        <f>C64</f>
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="F71">
+        <v>24</v>
+      </c>
+      <c r="I71">
+        <f>C55</f>
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <f>K70*2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="F72">
+        <v>36</v>
+      </c>
+      <c r="G72">
+        <f>C45</f>
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <f>C65</f>
+        <v>1.4349593495934958</v>
+      </c>
+      <c r="K72">
+        <f t="shared" ref="K72:K82" si="8">K71*2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="F73">
+        <v>48</v>
+      </c>
+      <c r="I73">
+        <f>C56</f>
+        <v>1.5203619909502262</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="F74">
+        <v>72</v>
+      </c>
+      <c r="G74">
+        <f>C46</f>
+        <v>1.9448818897637796</v>
+      </c>
+      <c r="H74">
+        <f>C66</f>
+        <v>2.1011904761904758</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="F75">
+        <v>96</v>
+      </c>
+      <c r="I75">
+        <f>C57</f>
+        <v>2.5074626865671643</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="8"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="F76">
+        <v>144</v>
+      </c>
+      <c r="G76">
+        <f>C47</f>
+        <v>3.4887005649717513</v>
+      </c>
+      <c r="H76">
+        <f>C67</f>
+        <v>3.0695652173913039</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="F77">
+        <v>192</v>
+      </c>
+      <c r="I77">
+        <f>C58</f>
+        <v>3.4250764525993884</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="8"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="F78">
+        <v>288</v>
+      </c>
+      <c r="G78">
+        <f>C48</f>
+        <v>7.1802325581395348</v>
+      </c>
+      <c r="H78">
+        <f>C68</f>
+        <v>3.4271844660194168</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="8"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="F79">
+        <v>384</v>
+      </c>
+      <c r="I79">
+        <f>C59</f>
+        <v>3.3802816901408455</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="8"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="F80">
+        <v>576</v>
+      </c>
+      <c r="G80">
+        <f>C49</f>
+        <v>13.646408839779005</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="8"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="81" spans="6:11">
+      <c r="F81">
+        <v>768</v>
+      </c>
+      <c r="I81">
+        <f>C60</f>
+        <v>3.4854771784232366</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="8"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="82" spans="6:11">
+      <c r="F82">
+        <v>1152</v>
+      </c>
+      <c r="G82">
+        <f>C50</f>
+        <v>15.632911392405061</v>
+      </c>
+      <c r="J82">
+        <v>4096</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="8"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="87" spans="6:11">
+      <c r="F87" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="6:11">
+      <c r="F88" s="5">
+        <v>18</v>
+      </c>
+      <c r="G88" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="6:11">
+      <c r="F89" s="8">
+        <v>36</v>
+      </c>
+      <c r="G89" s="8">
+        <v>0.7174796747967479</v>
+      </c>
+    </row>
+    <row r="90" spans="6:11">
+      <c r="F90" s="8">
+        <v>72</v>
+      </c>
+      <c r="G90" s="8">
+        <v>0.52529761904761896</v>
+      </c>
+    </row>
+    <row r="91" spans="6:11">
+      <c r="F91" s="8">
+        <v>144</v>
+      </c>
+      <c r="G91" s="8">
+        <v>0.38369565217391299</v>
+      </c>
+    </row>
+    <row r="92" spans="6:11">
+      <c r="F92" s="8">
+        <v>288</v>
+      </c>
+      <c r="G92" s="8">
+        <v>0.21419902912621355</v>
+      </c>
+    </row>
+    <row r="93" spans="6:11">
+      <c r="F93" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="12"/>
+      <c r="B98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I98" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="5">
+        <v>1</v>
+      </c>
+      <c r="B99" s="9">
+        <v>36</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" s="5">
+        <v>1</v>
+      </c>
+      <c r="E99" s="5">
+        <v>24</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" s="5">
+        <v>1</v>
+      </c>
+      <c r="H99" s="5">
+        <v>18</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="8">
+        <v>2</v>
+      </c>
+      <c r="B100" s="7">
+        <v>72</v>
+      </c>
+      <c r="C100">
+        <v>1.9448818897637796</v>
+      </c>
+      <c r="D100" s="8">
+        <v>0.97244094488188981</v>
+      </c>
+      <c r="E100" s="8">
+        <v>48</v>
+      </c>
+      <c r="F100">
+        <v>1.5203619909502262</v>
+      </c>
+      <c r="G100" s="8">
+        <v>0.76018099547511309</v>
+      </c>
+      <c r="H100" s="8">
+        <v>36</v>
+      </c>
+      <c r="I100">
+        <v>1.4349593495934958</v>
+      </c>
+      <c r="J100" s="8">
+        <v>0.7174796747967479</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="8">
+        <v>3</v>
+      </c>
+      <c r="B101" s="7">
+        <v>144</v>
+      </c>
+      <c r="C101">
+        <v>3.4887005649717513</v>
+      </c>
+      <c r="D101" s="8">
+        <v>0.87217514124293782</v>
+      </c>
+      <c r="E101" s="8">
+        <v>96</v>
+      </c>
+      <c r="F101">
+        <v>2.5074626865671643</v>
+      </c>
+      <c r="G101" s="8">
+        <v>0.62686567164179108</v>
+      </c>
+      <c r="H101" s="8">
+        <v>72</v>
+      </c>
+      <c r="I101">
+        <v>2.1011904761904758</v>
+      </c>
+      <c r="J101" s="8">
+        <v>0.52529761904761896</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="8">
+        <v>4</v>
+      </c>
+      <c r="B102" s="7">
+        <v>288</v>
+      </c>
+      <c r="C102">
+        <v>7.1802325581395348</v>
+      </c>
+      <c r="D102" s="8">
+        <v>0.89752906976744184</v>
+      </c>
+      <c r="E102" s="8">
+        <v>192</v>
+      </c>
+      <c r="F102">
+        <v>3.4250764525993884</v>
+      </c>
+      <c r="G102" s="8">
+        <v>0.42813455657492355</v>
+      </c>
+      <c r="H102" s="8">
+        <v>144</v>
+      </c>
+      <c r="I102">
+        <v>3.0695652173913039</v>
+      </c>
+      <c r="J102" s="8">
+        <v>0.38369565217391299</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="8">
+        <v>5</v>
+      </c>
+      <c r="B103" s="7">
+        <v>576</v>
+      </c>
+      <c r="C103">
+        <v>13.646408839779005</v>
+      </c>
+      <c r="D103" s="8">
+        <v>0.85290055248618779</v>
+      </c>
+      <c r="E103" s="8">
+        <v>384</v>
+      </c>
+      <c r="F103">
+        <v>3.3802816901408455</v>
+      </c>
+      <c r="G103" s="8">
+        <v>0.21126760563380281</v>
+      </c>
+      <c r="H103" s="8">
+        <v>288</v>
+      </c>
+      <c r="I103">
+        <v>3.4271844660194168</v>
+      </c>
+      <c r="J103" s="8">
+        <v>0.21419902912621355</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="6">
+        <v>6</v>
+      </c>
+      <c r="B104" s="10">
+        <v>1152</v>
+      </c>
+      <c r="C104">
+        <v>15.632911392405061</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0.48852848101265817</v>
+      </c>
+      <c r="E104" s="6">
+        <v>768</v>
+      </c>
+      <c r="F104">
+        <v>3.4854771784232366</v>
+      </c>
+      <c r="G104" s="6">
+        <v>0.10892116182572614</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J104" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="15">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="H97:J97"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1473,4 +3669,121 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f>$B$6 / B6</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>(C6/A6) *$A$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C10" si="0">$B$6 / B7</f>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D10" si="1">(C7/A7) *$A$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.3125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update performance analysis - pRicing
</commit_message>
<xml_diff>
--- a/documents/resources/evaluation/performance/Performance-Graphs.xlsx
+++ b/documents/resources/evaluation/performance/Performance-Graphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
   <si>
     <t>INDY2</t>
   </si>
@@ -43,9 +43,6 @@
     <t>#Compute node</t>
   </si>
   <si>
-    <t>Perf Delta</t>
-  </si>
-  <si>
     <t>Simulation time</t>
   </si>
   <si>
@@ -58,16 +55,7 @@
     <t>Time / s</t>
   </si>
   <si>
-    <t>Core count</t>
-  </si>
-  <si>
-    <t>Execution time</t>
-  </si>
-  <si>
     <t>Speed up</t>
-  </si>
-  <si>
-    <t>Efficienc</t>
   </si>
   <si>
     <t>EFFICIENCY</t>
@@ -96,6 +84,57 @@
   <si>
     <t>Ideal parallel 
 efficiency</t>
+  </si>
+  <si>
+    <t>AWS-EC2vINDY2 Perf Delta</t>
+  </si>
+  <si>
+    <t>AWS-EC2vARCHER Perf Delta</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Partner Price</t>
+  </si>
+  <si>
+    <t>Non Partner price</t>
+  </si>
+  <si>
+    <t>Time (in hour)</t>
+  </si>
+  <si>
+    <t>ARCHER compute nodes</t>
+  </si>
+  <si>
+    <t>Time ratio</t>
+  </si>
+  <si>
+    <t>Simulation cost</t>
+  </si>
+  <si>
+    <t>Compute node</t>
+  </si>
+  <si>
+    <t>Base price</t>
+  </si>
+  <si>
+    <t>Time different ratio</t>
+  </si>
+  <si>
+    <t>Time difference ratio</t>
+  </si>
+  <si>
+    <t>ARCHER simulation cost</t>
+  </si>
+  <si>
+    <t>AWS EC2 simulation cost</t>
+  </si>
+  <si>
+    <t>ARCHER-partner</t>
+  </si>
+  <si>
+    <t>ARCHER-nonpartner</t>
   </si>
 </sst>
 </file>
@@ -234,7 +273,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,8 +511,90 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,8 +650,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="319">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -649,6 +776,47 @@
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -767,6 +935,47 @@
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1764,6 +1973,342 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARCHER-partner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$36:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$36:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.263095238095238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.319047619047619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.467142857142857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.946666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.836190476190476</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ARCHER-nonpartner</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$36:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$36:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.631428571428571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.765714285714286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.121142857142857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.271999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.406857142857142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AWS-EC2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$36:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$36:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.58639880952381</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.211071428571429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.134523809523809</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.406190476190477</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2090176984"/>
+        <c:axId val="-2093005080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2090176984"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Compute</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> node(log2)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2093005080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2093005080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Simulation</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Cost</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2090176984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1821,6 +2366,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2153,13 +2733,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
@@ -2325,28 +2906,28 @@
     </row>
     <row r="21" spans="1:8">
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F22" t="s">
-        <v>7</v>
+      <c r="F22" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2458,6 +3039,10 @@
         <f t="shared" si="1"/>
         <v>5.6906077348066297</v>
       </c>
+      <c r="G27">
+        <f>1.81*569.0607735%</f>
+        <v>10.30000000035</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="C28">
@@ -2469,7 +3054,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>0</v>
@@ -2488,22 +3073,22 @@
     <row r="33" spans="1:11">
       <c r="A33" s="12"/>
       <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="D33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="F33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2554,7 +3139,7 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B36" s="7">
         <v>144</v>
@@ -2577,7 +3162,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B37" s="7">
         <v>288</v>
@@ -2600,7 +3185,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="8">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B38" s="7">
         <v>576</v>
@@ -2623,7 +3208,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="6">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B39" s="10">
         <v>1152</v>
@@ -2646,29 +3231,29 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="G43" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="45">
       <c r="A44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F44" t="s">
         <v>4</v>
@@ -2683,10 +3268,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2864,7 +3449,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2883,16 +3468,16 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F54">
         <v>384</v>
@@ -3027,7 +3612,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -3035,16 +3620,16 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" t="s">
         <v>11</v>
       </c>
-      <c r="C63" t="s">
-        <v>14</v>
-      </c>
       <c r="D63" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3127,7 +3712,7 @@
         <v>0.21419902912621355</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -3148,10 +3733,10 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K69" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3346,10 +3931,10 @@
     </row>
     <row r="87" spans="6:11">
       <c r="F87" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="6:11">
@@ -3402,7 +3987,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B97" s="13" t="s">
         <v>0</v>
@@ -3423,31 +4008,31 @@
     <row r="98" spans="1:10">
       <c r="A98" s="12"/>
       <c r="B98" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D98" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E98" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F98" s="17" t="s">
-        <v>23</v>
-      </c>
       <c r="G98" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I98" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H98" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I98" s="17" t="s">
-        <v>23</v>
-      </c>
       <c r="J98" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3673,113 +4258,767 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:Q48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
+    <row r="5" spans="1:17">
+      <c r="A5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <f>$B$6 / B6</f>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="12"/>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="D6">
-        <f>(C6/A6) *$A$6</f>
+      <c r="B7" s="8">
+        <v>33.6</v>
+      </c>
+      <c r="C7" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
+      <c r="D7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.48</v>
+      </c>
+      <c r="F7" s="8">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G7">
+        <f>F7/$B$7</f>
+        <v>1.0505952380952379</v>
+      </c>
+      <c r="H7" s="20">
+        <v>1.51</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <v>22.1</v>
+      </c>
+      <c r="C8" s="7">
+        <f>B8/$B$7</f>
+        <v>0.65773809523809523</v>
+      </c>
+      <c r="D8" s="1">
+        <f>$D$7*A8</f>
+        <v>0.4</v>
+      </c>
+      <c r="E8" s="8">
+        <f>$E$7 *A8</f>
+        <v>0.96</v>
+      </c>
+      <c r="F8" s="8">
+        <v>24.6</v>
+      </c>
+      <c r="G8">
+        <f>F8/$B$7</f>
+        <v>0.73214285714285721</v>
+      </c>
+      <c r="H8" s="8">
+        <f>$H$7 *A8</f>
+        <v>3.02</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ref="C7:C10" si="0">$B$6 / B7</f>
+      <c r="P8">
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="8">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>13.4</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9:C12" si="0">B9/$B$7</f>
+        <v>0.39880952380952378</v>
+      </c>
+      <c r="D9" s="1">
+        <f>$D$7*A9</f>
+        <v>0.8</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" ref="E9:E12" si="1">$E$7 *A9</f>
+        <v>1.92</v>
+      </c>
+      <c r="F9" s="8">
+        <v>16.8</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G11" si="2">F9/$B$7</f>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="8">
+        <f>$H$7 *A9</f>
+        <v>6.04</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0.2</v>
+      </c>
+      <c r="N9">
+        <v>0.4</v>
+      </c>
+      <c r="O9">
+        <v>0.8</v>
+      </c>
+      <c r="P9">
+        <v>1.6</v>
+      </c>
+      <c r="Q9">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9.81</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.29196428571428573</v>
+      </c>
+      <c r="D10" s="1">
+        <f>$D$7*A10</f>
+        <v>1.6</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="1"/>
+        <v>3.84</v>
+      </c>
+      <c r="F10" s="8">
+        <v>11.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.34226190476190477</v>
+      </c>
+      <c r="H10" s="8">
+        <f>$H$7 *A10</f>
+        <v>12.08</v>
+      </c>
+      <c r="L10">
         <v>2</v>
       </c>
-      <c r="D7">
-        <f t="shared" ref="D7:D10" si="1">(C7/A7) *$A$6</f>
+      <c r="M10">
+        <f>$C$7*L10*$D$7</f>
+        <v>0.4</v>
+      </c>
+      <c r="N10">
+        <f>$C$8*L10*$D$8</f>
+        <v>0.52619047619047621</v>
+      </c>
+      <c r="O10">
+        <f>$C$9*$L10*$D$9</f>
+        <v>0.63809523809523805</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ref="P10:Q10" si="3">$C$9*$L10*$D$9</f>
+        <v>0.63809523809523805</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>0.63809523809523805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="8">
+        <v>16</v>
+      </c>
+      <c r="B11" s="8">
+        <v>9.94</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.29583333333333328</v>
+      </c>
+      <c r="D11" s="1">
+        <f>$D$7*A11</f>
+        <v>3.2</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="1"/>
+        <v>7.68</v>
+      </c>
+      <c r="F11" s="8">
+        <v>10.3</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0.30654761904761907</v>
+      </c>
+      <c r="H11" s="8">
+        <f>$H$7 *A11</f>
+        <v>24.16</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11:M15" si="4">$C$7*L11*$D$7</f>
+        <v>0.8</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:N15" si="5">$C$8*L11*$D$8</f>
+        <v>1.0523809523809524</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11:O15" si="6">$C$9*$L11*$D$9</f>
+        <v>1.2761904761904761</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="6">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6">
+        <v>9.64</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.28690476190476188</v>
+      </c>
+      <c r="D12" s="6">
+        <f>$D$7*A12</f>
+        <v>6.4</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="1"/>
+        <v>15.36</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="6">
+        <f>$H$7 *A12</f>
+        <v>48.32</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>2.1047619047619048</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>2.5523809523809522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="L13">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>3.2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>4.2095238095238097</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>5.1047619047619044</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="L14">
+        <v>32</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="4"/>
+        <v>6.4</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="5"/>
+        <v>8.4190476190476193</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="6"/>
+        <v>10.209523809523809</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="L15">
+        <v>64</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="4"/>
+        <v>12.8</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>16.838095238095239</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>20.419047619047618</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="B25">
+        <v>0.2</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>A25*$B$25*A25</f>
+        <v>0.2</v>
+      </c>
+      <c r="E25">
+        <f>A25*$B$26*C25</f>
+        <v>0.48</v>
+      </c>
+      <c r="F25" s="19">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f>A25*$B$27*F25</f>
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>0.48</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.65773809523809523</v>
+      </c>
+      <c r="D26">
+        <f>A26*$B$25*C26</f>
+        <v>0.2630952380952381</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E30" si="7">A26*$B$26*C26</f>
+        <v>0.63142857142857145</v>
+      </c>
+      <c r="F26">
+        <v>0.69688385269121822</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="8">A26*$B$27*F26</f>
+        <v>2.1045892351274791</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>1.51</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.39880952380952378</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:D30" si="9">A27*$B$25*C27</f>
+        <v>0.31904761904761902</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="7"/>
+        <v>0.76571428571428568</v>
+      </c>
+      <c r="F27">
+        <v>0.47592067988668563</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="8"/>
+        <v>2.874560906515581</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
+      <c r="C28" s="7">
+        <v>0.29196428571428573</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="9"/>
+        <v>0.46714285714285719</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="7"/>
+        <v>1.1211428571428572</v>
+      </c>
+      <c r="F28">
+        <v>0.3257790368271955</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="8"/>
+        <v>3.9354107648725218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.29583333333333328</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="9"/>
+        <v>0.94666666666666655</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="7"/>
+        <v>2.2719999999999994</v>
+      </c>
+      <c r="F29">
+        <v>0.29178470254957511</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="8"/>
+        <v>7.0495184135977347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>32</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.28690476190476188</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="9"/>
+        <v>1.8361904761904762</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="7"/>
+        <v>4.4068571428571426</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G26:G30" si="10">C30*$B$27*F30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="B34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
         <v>2</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <f>0.2*A36*B36</f>
+        <v>0.2</v>
+      </c>
+      <c r="D36">
+        <f>0.48*A36*B36</f>
+        <v>0.48</v>
+      </c>
+      <c r="E36" s="19">
+        <v>1.0505952380952379</v>
+      </c>
+      <c r="F36">
+        <f>1.51*E36*A36</f>
+        <v>1.5863988095238093</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>0.65773809523809523</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ref="C37:C41" si="11">0.2*A37*B37</f>
+        <v>0.2630952380952381</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:D41" si="12">0.48*A37*B37</f>
+        <v>0.63142857142857145</v>
+      </c>
+      <c r="E37">
+        <v>0.73214285714285721</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ref="F37:F40" si="13">1.51*E37*A37</f>
+        <v>2.2110714285714286</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0.39880952380952378</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="11"/>
+        <v>0.31904761904761902</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="12"/>
+        <v>0.76571428571428568</v>
+      </c>
+      <c r="E38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="F38">
+        <f t="shared" si="13"/>
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>0.29196428571428573</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="11"/>
+        <v>0.46714285714285719</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="12"/>
+        <v>1.1211428571428572</v>
+      </c>
+      <c r="E39">
+        <v>0.34226190476190477</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="13"/>
+        <v>4.1345238095238095</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="B40">
+        <v>0.29583333333333328</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="11"/>
+        <v>0.94666666666666655</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="12"/>
+        <v>2.2719999999999994</v>
+      </c>
+      <c r="E40">
+        <v>0.30654761904761907</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="13"/>
+        <v>7.4061904761904769</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
         <v>32</v>
       </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>0.3125</v>
+      <c r="B41">
+        <v>0.28690476190476188</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="11"/>
+        <v>1.8361904761904762</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="12"/>
+        <v>4.4068571428571426</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="E44">
+        <f>F36/C36</f>
+        <v>7.931994047619046</v>
+      </c>
+      <c r="F44">
+        <f>F36/D36</f>
+        <v>3.3049975198412693</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="E45">
+        <f>F37/C37</f>
+        <v>8.4040723981900456</v>
+      </c>
+      <c r="F45">
+        <f>F37/D37</f>
+        <v>3.5016968325791855</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="E46">
+        <f>F38/C38</f>
+        <v>9.4656716417910456</v>
+      </c>
+      <c r="F46">
+        <f>F38/D38</f>
+        <v>3.944029850746269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="E47">
+        <f>F39/C39</f>
+        <v>8.8506625891946982</v>
+      </c>
+      <c r="F47">
+        <f>F39/D39</f>
+        <v>3.6877760788311242</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="E48">
+        <f>F40/C40</f>
+        <v>7.8234406438631812</v>
+      </c>
+      <c r="F48">
+        <f>F40/D40</f>
+        <v>3.2597669349429923</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>